<commit_message>
Updated planned of Release and Artifact List to 2380 and 700 respectivly
</commit_message>
<xml_diff>
--- a/blueprint-jira-better-excel/_Current-Release-Dashboard.xlsx
+++ b/blueprint-jira-better-excel/_Current-Release-Dashboard.xlsx
@@ -35,7 +35,7 @@
   </definedNames>
   <calcPr calcId="171027"/>
   <pivotCaches>
-    <pivotCache cacheId="102" r:id="rId18"/>
+    <pivotCache cacheId="12" r:id="rId18"/>
   </pivotCaches>
   <fileRecoveryPr autoRecover="0"/>
 </workbook>
@@ -1760,10 +1760,10 @@
                 <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0" formatCode="0%">
-                  <c:v>0.63793103448275867</c:v>
+                  <c:v>0.64655172413793105</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.36206896551724133</c:v>
+                  <c:v>0.35344827586206895</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5236,10 +5236,10 @@
                 <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0" formatCode="0%">
-                  <c:v>0.63793103448275867</c:v>
+                  <c:v>0.64655172413793105</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.36206896551724133</c:v>
+                  <c:v>0.35344827586206895</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7245,46 +7245,46 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>675</c:v>
+                  <c:v>700</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>645.90517241379314</c:v>
+                  <c:v>669.82758620689651</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>587.7155172413793</c:v>
+                  <c:v>609.48275862068965</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>529.52586206896558</c:v>
+                  <c:v>549.13793103448279</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>477.15517241379308</c:v>
+                  <c:v>494.82758620689651</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>418.9655172413793</c:v>
+                  <c:v>434.48275862068965</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>360.77586206896558</c:v>
+                  <c:v>374.13793103448279</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>308.40517241379308</c:v>
+                  <c:v>319.82758620689651</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>308.40517241379308</c:v>
+                  <c:v>319.82758620689651</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>250.21551724137933</c:v>
+                  <c:v>259.48275862068965</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>197.84482758620692</c:v>
+                  <c:v>205.17241379310346</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>139.65517241379308</c:v>
+                  <c:v>144.82758620689654</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>87.284482758620683</c:v>
+                  <c:v>90.517241379310335</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>29.094827586206918</c:v>
+                  <c:v>30.17241379310347</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>0</c:v>
@@ -8548,49 +8548,49 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>675</c:v>
+                  <c:v>700</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>675</c:v>
+                  <c:v>700</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>675</c:v>
+                  <c:v>700</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>675</c:v>
+                  <c:v>700</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>675</c:v>
+                  <c:v>700</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>675</c:v>
+                  <c:v>700</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>675</c:v>
+                  <c:v>700</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>675</c:v>
+                  <c:v>700</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>675</c:v>
+                  <c:v>700</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>675</c:v>
+                  <c:v>700</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>675</c:v>
+                  <c:v>700</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>675</c:v>
+                  <c:v>700</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>675</c:v>
+                  <c:v>700</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>675</c:v>
+                  <c:v>700</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>675</c:v>
+                  <c:v>700</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -23785,46 +23785,46 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>2350</c:v>
+                  <c:v>2380</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2248.7068965517242</c:v>
+                  <c:v>2277.4137931034484</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2046.1206896551726</c:v>
+                  <c:v>2072.2413793103447</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1843.5344827586209</c:v>
+                  <c:v>1867.0689655172416</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1661.206896551724</c:v>
+                  <c:v>1682.4137931034481</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1458.6206896551726</c:v>
+                  <c:v>1477.2413793103449</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1256.0344827586209</c:v>
+                  <c:v>1272.0689655172416</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1073.706896551724</c:v>
+                  <c:v>1087.4137931034481</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1073.706896551724</c:v>
+                  <c:v>1087.4137931034481</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>871.12068965517244</c:v>
+                  <c:v>882.24137931034488</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>688.79310344827593</c:v>
+                  <c:v>697.58620689655174</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>486.20689655172407</c:v>
+                  <c:v>492.4137931034482</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>303.87931034482756</c:v>
+                  <c:v>307.75862068965512</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>101.29310344827593</c:v>
+                  <c:v>102.5862068965518</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>0</c:v>
@@ -25080,49 +25080,49 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>2350</c:v>
+                  <c:v>2380</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2350</c:v>
+                  <c:v>2380</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2350</c:v>
+                  <c:v>2380</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2350</c:v>
+                  <c:v>2380</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2350</c:v>
+                  <c:v>2380</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2350</c:v>
+                  <c:v>2380</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2350</c:v>
+                  <c:v>2380</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2350</c:v>
+                  <c:v>2380</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2350</c:v>
+                  <c:v>2380</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2350</c:v>
+                  <c:v>2380</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2350</c:v>
+                  <c:v>2380</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2350</c:v>
+                  <c:v>2380</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2350</c:v>
+                  <c:v>2380</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2350</c:v>
+                  <c:v>2380</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2350</c:v>
+                  <c:v>2380</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -25473,10 +25473,10 @@
                 <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0" formatCode="0%">
-                  <c:v>0.63793103448275867</c:v>
+                  <c:v>0.64655172413793105</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.36206896551724133</c:v>
+                  <c:v>0.35344827586206895</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -43164,7 +43164,7 @@
               <a:cs typeface="Calibri"/>
             </a:rPr>
             <a:pPr algn="ctr"/>
-            <a:t>64%</a:t>
+            <a:t>65%</a:t>
           </a:fld>
           <a:endParaRPr lang="en-US" sz="1800" b="1">
             <a:solidFill>
@@ -43840,7 +43840,7 @@
               <a:cs typeface="Calibri"/>
             </a:rPr>
             <a:pPr algn="ctr"/>
-            <a:t>64%</a:t>
+            <a:t>65%</a:t>
           </a:fld>
           <a:endParaRPr lang="en-US" sz="1800" b="1">
             <a:solidFill>
@@ -44347,7 +44347,7 @@
               <a:cs typeface="Calibri"/>
             </a:rPr>
             <a:pPr algn="ctr"/>
-            <a:t>64%</a:t>
+            <a:t>65%</a:t>
           </a:fld>
           <a:endParaRPr lang="en-US" sz="1800" b="1">
             <a:solidFill>
@@ -44364,7 +44364,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshOnLoad="1" refreshedBy="Alex Folomechine" refreshedDate="43313.64081597222" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="90">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshOnLoad="1" refreshedBy="Alex Folomechine" refreshedDate="43314.558741782406" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="90">
   <cacheSource type="worksheet">
     <worksheetSource name="issues"/>
   </cacheSource>
@@ -48803,8 +48803,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable9" cacheId="102" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="15">
-  <location ref="G24:H29" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="12" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="9">
+  <location ref="A24:B29" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
   <pivotFields count="46">
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField axis="axisPage" subtotalTop="0" multipleItemSelectionAllowed="1" showAll="0">
@@ -48827,15 +48827,7 @@
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisPage" subtotalTop="0" showAll="0">
-      <items count="5">
-        <item x="0"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField subtotalTop="0" showAll="0"/>
@@ -48903,10 +48895,9 @@
   <colItems count="1">
     <i/>
   </colItems>
-  <pageFields count="3">
+  <pageFields count="2">
     <pageField fld="32" item="2" hier="-1"/>
     <pageField fld="1" hier="-1"/>
-    <pageField fld="10" item="1" hier="-1"/>
   </pageFields>
   <dataFields count="5">
     <dataField name="Done" fld="44" baseField="0" baseItem="32"/>
@@ -48915,7 +48906,7 @@
     <dataField name="Ready" fld="39" baseField="0" baseItem="32"/>
     <dataField name="Not Decomposed" fld="45" baseField="0" baseItem="32"/>
   </dataFields>
-  <chartFormats count="27">
+  <chartFormats count="15">
     <chartFormat chart="0" format="7" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="2">
@@ -49057,114 +49048,6 @@
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="7" format="7" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="7" format="8">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="7" format="9">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="7" format="10">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="7" format="11">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="7" format="12">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="4"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="14" format="19" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="14" format="20">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="14" format="21">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="14" format="22">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="14" format="23">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="14" format="24">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="4"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
   </chartFormats>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -49179,98 +49062,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable10.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable5" cacheId="102" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="B3:C5" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="46">
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisRow" subtotalTop="0" showAll="0">
-      <items count="8">
-        <item h="1" x="0"/>
-        <item h="1" x="6"/>
-        <item x="2"/>
-        <item h="1" x="4"/>
-        <item h="1" x="3"/>
-        <item h="1" x="5"/>
-        <item h="1" x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField dataField="1" subtotalTop="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="1"/>
-  </rowFields>
-  <rowItems count="2">
-    <i>
-      <x v="2"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Sum of Epic Not Decomposed Estimate" fld="45" baseField="1" baseItem="2"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable11.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable7" cacheId="102" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable7" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="B12:B13" firstHeaderRow="1" firstDataRow="1" firstDataCol="0" rowPageCount="2" colPageCount="1"/>
   <pivotFields count="46">
     <pivotField subtotalTop="0" showAll="0"/>
@@ -49406,8 +49198,1066 @@
 </pivotTableDefinition>
 </file>
 
+<file path=xl/pivotTables/pivotTable11.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable5" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="B3:C5" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="46">
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisRow" subtotalTop="0" showAll="0">
+      <items count="8">
+        <item h="1" x="0"/>
+        <item h="1" x="6"/>
+        <item x="2"/>
+        <item h="1" x="4"/>
+        <item h="1" x="3"/>
+        <item h="1" x="5"/>
+        <item h="1" x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dataField="1" subtotalTop="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="2">
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Epic Not Decomposed Estimate" fld="45" baseField="1" baseItem="2"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
 <file path=xl/pivotTables/pivotTable12.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="102" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="11">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="15">
+  <location ref="G5:H11" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
+  <pivotFields count="46">
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisPage" subtotalTop="0" multipleItemSelectionAllowed="1" showAll="0">
+      <items count="8">
+        <item h="1" x="0"/>
+        <item h="1" x="6"/>
+        <item h="1" x="2"/>
+        <item x="4"/>
+        <item x="3"/>
+        <item x="5"/>
+        <item h="1" x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisPage" subtotalTop="0" showAll="0">
+      <items count="5">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisRow" subtotalTop="0" showAll="0">
+      <items count="10">
+        <item h="1" x="0"/>
+        <item h="1" x="7"/>
+        <item x="6"/>
+        <item x="5"/>
+        <item x="4"/>
+        <item x="3"/>
+        <item x="2"/>
+        <item h="1" x="8"/>
+        <item h="1" x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisPage" subtotalTop="0" showAll="0">
+      <items count="12">
+        <item x="0"/>
+        <item x="6"/>
+        <item x="10"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="9"/>
+        <item x="4"/>
+        <item x="8"/>
+        <item x="5"/>
+        <item x="7"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField subtotalTop="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="34"/>
+  </rowFields>
+  <rowItems count="6">
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <pageFields count="3">
+    <pageField fld="32" item="2" hier="-1"/>
+    <pageField fld="1" hier="-1"/>
+    <pageField fld="37" item="4" hier="-1"/>
+  </pageFields>
+  <dataFields count="1">
+    <dataField name="Sum of Story Points" fld="13" baseField="34" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="32">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="37" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="1" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="2">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="34" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="3">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="34" count="1" selected="0">
+            <x v="6"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="4">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="34" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="5">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="34" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="11" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="12">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="34" count="1" selected="0">
+            <x v="6"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="13">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="34" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="14">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="34" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="15">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="34" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="16" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="17">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="34" count="1" selected="0">
+            <x v="6"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="18">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="34" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="19">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="34" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="20">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="34" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="4" format="21" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="4" format="22">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="34" count="1" selected="0">
+            <x v="6"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="4" format="23">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="34" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="4" format="24">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="34" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="4" format="25">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="34" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="11" format="56" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="11" format="57">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="34" count="1" selected="0">
+            <x v="6"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="11" format="58">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="34" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="11" format="59">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="34" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="11" format="60">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="34" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="14" format="10" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="14" format="11">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="34" count="1" selected="0">
+            <x v="6"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="14" format="12">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="34" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="14" format="13">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="34" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="14" format="14">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="34" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="14" format="15">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="34" count="1" selected="0">
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable13.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="16">
+  <location ref="D5:E11" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
+  <pivotFields count="46">
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisPage" subtotalTop="0" multipleItemSelectionAllowed="1" showAll="0">
+      <items count="8">
+        <item h="1" x="0"/>
+        <item h="1" x="6"/>
+        <item h="1" x="2"/>
+        <item x="4"/>
+        <item x="3"/>
+        <item x="5"/>
+        <item h="1" x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisPage" subtotalTop="0" showAll="0">
+      <items count="5">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisRow" subtotalTop="0" showAll="0">
+      <items count="10">
+        <item h="1" x="0"/>
+        <item h="1" x="7"/>
+        <item x="6"/>
+        <item x="5"/>
+        <item x="4"/>
+        <item h="1" x="8"/>
+        <item h="1" x="1"/>
+        <item x="3"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisPage" subtotalTop="0" showAll="0">
+      <items count="12">
+        <item x="0"/>
+        <item x="6"/>
+        <item x="10"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="9"/>
+        <item x="4"/>
+        <item x="8"/>
+        <item x="5"/>
+        <item x="7"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField subtotalTop="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="34"/>
+  </rowFields>
+  <rowItems count="6">
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <pageFields count="3">
+    <pageField fld="32" item="2" hier="-1"/>
+    <pageField fld="1" hier="-1"/>
+    <pageField fld="37" item="3" hier="-1"/>
+  </pageFields>
+  <dataFields count="1">
+    <dataField name="Sum of Story Points" fld="13" baseField="34" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="27">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="37" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="1" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="2">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="34" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="3">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="34" count="1" selected="0">
+            <x v="8"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="4">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="34" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="5">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="34" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="11" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="12">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="34" count="1" selected="0">
+            <x v="8"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="13">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="34" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="14">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="34" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="15">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="34" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="16" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="17">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="34" count="1" selected="0">
+            <x v="8"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="18">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="34" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="19">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="34" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="20">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="34" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="4" format="21" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="4" format="22">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="34" count="1" selected="0">
+            <x v="8"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="4" format="23">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="34" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="4" format="24">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="34" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="4" format="25">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="34" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="15" format="66" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="15" format="67">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="34" count="1" selected="0">
+            <x v="8"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="15" format="68">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="34" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="15" format="69">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="34" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="15" format="70">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="34" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="15" format="71">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="34" count="1" selected="0">
+            <x v="7"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable14.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="11">
   <location ref="A5:B11" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
   <pivotFields count="46">
     <pivotField subtotalTop="0" showAll="0"/>
@@ -49621,8 +50471,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable13.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable5" cacheId="102" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="15">
+<file path=xl/pivotTables/pivotTable15.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable5" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="15">
   <location ref="J5:K11" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
   <pivotFields count="46">
     <pivotField subtotalTop="0" showAll="0"/>
@@ -50133,975 +50983,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable14.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="102" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="15">
-  <location ref="G5:H11" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
-  <pivotFields count="46">
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisPage" subtotalTop="0" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="8">
-        <item h="1" x="0"/>
-        <item h="1" x="6"/>
-        <item h="1" x="2"/>
-        <item x="4"/>
-        <item x="3"/>
-        <item x="5"/>
-        <item h="1" x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisPage" subtotalTop="0" showAll="0">
-      <items count="5">
-        <item x="0"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisRow" subtotalTop="0" showAll="0">
-      <items count="10">
-        <item h="1" x="0"/>
-        <item h="1" x="7"/>
-        <item x="6"/>
-        <item x="5"/>
-        <item x="4"/>
-        <item x="3"/>
-        <item x="2"/>
-        <item h="1" x="8"/>
-        <item h="1" x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisPage" subtotalTop="0" showAll="0">
-      <items count="12">
-        <item x="0"/>
-        <item x="6"/>
-        <item x="10"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="9"/>
-        <item x="4"/>
-        <item x="8"/>
-        <item x="5"/>
-        <item x="7"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField subtotalTop="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="34"/>
-  </rowFields>
-  <rowItems count="6">
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <pageFields count="3">
-    <pageField fld="32" item="2" hier="-1"/>
-    <pageField fld="1" hier="-1"/>
-    <pageField fld="37" item="4" hier="-1"/>
-  </pageFields>
-  <dataFields count="1">
-    <dataField name="Sum of Story Points" fld="13" baseField="34" baseItem="0"/>
-  </dataFields>
-  <chartFormats count="32">
-    <chartFormat chart="0" format="0" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="37" count="1" selected="0">
-            <x v="4"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="1" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="2">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="34" count="1" selected="0">
-            <x v="4"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="3">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="34" count="1" selected="0">
-            <x v="6"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="4">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="34" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="5">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="34" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="2" format="11" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="2" format="12">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="34" count="1" selected="0">
-            <x v="6"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="2" format="13">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="34" count="1" selected="0">
-            <x v="4"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="2" format="14">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="34" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="2" format="15">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="34" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="3" format="16" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="3" format="17">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="34" count="1" selected="0">
-            <x v="6"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="3" format="18">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="34" count="1" selected="0">
-            <x v="4"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="3" format="19">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="34" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="3" format="20">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="34" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="4" format="21" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="4" format="22">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="34" count="1" selected="0">
-            <x v="6"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="4" format="23">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="34" count="1" selected="0">
-            <x v="4"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="4" format="24">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="34" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="4" format="25">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="34" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="11" format="56" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="11" format="57">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="34" count="1" selected="0">
-            <x v="6"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="11" format="58">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="34" count="1" selected="0">
-            <x v="4"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="11" format="59">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="34" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="11" format="60">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="34" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="14" format="10" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="14" format="11">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="34" count="1" selected="0">
-            <x v="6"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="14" format="12">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="34" count="1" selected="0">
-            <x v="4"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="14" format="13">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="34" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="14" format="14">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="34" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="14" format="15">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="34" count="1" selected="0">
-            <x v="5"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable15.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="102" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="16">
-  <location ref="D5:E11" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
-  <pivotFields count="46">
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisPage" subtotalTop="0" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="8">
-        <item h="1" x="0"/>
-        <item h="1" x="6"/>
-        <item h="1" x="2"/>
-        <item x="4"/>
-        <item x="3"/>
-        <item x="5"/>
-        <item h="1" x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisPage" subtotalTop="0" showAll="0">
-      <items count="5">
-        <item x="0"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisRow" subtotalTop="0" showAll="0">
-      <items count="10">
-        <item h="1" x="0"/>
-        <item h="1" x="7"/>
-        <item x="6"/>
-        <item x="5"/>
-        <item x="4"/>
-        <item h="1" x="8"/>
-        <item h="1" x="1"/>
-        <item x="3"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisPage" subtotalTop="0" showAll="0">
-      <items count="12">
-        <item x="0"/>
-        <item x="6"/>
-        <item x="10"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="9"/>
-        <item x="4"/>
-        <item x="8"/>
-        <item x="5"/>
-        <item x="7"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField subtotalTop="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="34"/>
-  </rowFields>
-  <rowItems count="6">
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <pageFields count="3">
-    <pageField fld="32" item="2" hier="-1"/>
-    <pageField fld="1" hier="-1"/>
-    <pageField fld="37" item="3" hier="-1"/>
-  </pageFields>
-  <dataFields count="1">
-    <dataField name="Sum of Story Points" fld="13" baseField="34" baseItem="0"/>
-  </dataFields>
-  <chartFormats count="27">
-    <chartFormat chart="0" format="0" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="37" count="1" selected="0">
-            <x v="4"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="1" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="2">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="34" count="1" selected="0">
-            <x v="4"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="3">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="34" count="1" selected="0">
-            <x v="8"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="4">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="34" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="5">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="34" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="2" format="11" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="2" format="12">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="34" count="1" selected="0">
-            <x v="8"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="2" format="13">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="34" count="1" selected="0">
-            <x v="4"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="2" format="14">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="34" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="2" format="15">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="34" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="3" format="16" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="3" format="17">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="34" count="1" selected="0">
-            <x v="8"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="3" format="18">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="34" count="1" selected="0">
-            <x v="4"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="3" format="19">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="34" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="3" format="20">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="34" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="4" format="21" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="4" format="22">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="34" count="1" selected="0">
-            <x v="8"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="4" format="23">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="34" count="1" selected="0">
-            <x v="4"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="4" format="24">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="34" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="4" format="25">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="34" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="15" format="66" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="15" format="67">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="34" count="1" selected="0">
-            <x v="8"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="15" format="68">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="34" count="1" selected="0">
-            <x v="4"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="15" format="69">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="34" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="15" format="70">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="34" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="15" format="71">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="34" count="1" selected="0">
-            <x v="7"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
 <file path=xl/pivotTables/pivotTable16.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="102" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
   <location ref="B4:H20" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
   <pivotFields count="46">
     <pivotField subtotalTop="0" showAll="0"/>
@@ -51403,7 +51286,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable17.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="102" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="D4:E11" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
   <pivotFields count="46">
     <pivotField subtotalTop="0" showAll="0"/>
@@ -51670,7 +51553,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable18.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="102" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="F8:L11" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
   <pivotFields count="46">
     <pivotField dataField="1" subtotalTop="0" showAll="0"/>
@@ -51983,7 +51866,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable19.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="102" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="5">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="5">
   <location ref="B9:C15" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="4" colPageCount="1"/>
   <pivotFields count="46">
     <pivotField dataField="1" subtotalTop="0" showAll="0"/>
@@ -52385,8 +52268,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable5" cacheId="102" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
-  <location ref="D35:D36" firstHeaderRow="1" firstDataRow="1" firstDataCol="0" rowPageCount="3" colPageCount="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="Y4:AA8" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
   <pivotFields count="46">
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField axis="axisPage" subtotalTop="0" multipleItemSelectionAllowed="1" showAll="0">
@@ -52409,12 +52292,12 @@
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisPage" subtotalTop="0" showAll="0">
+    <pivotField axis="axisRow" subtotalTop="0" showAll="0">
       <items count="5">
         <item x="0"/>
+        <item x="1"/>
         <item x="2"/>
         <item x="3"/>
-        <item x="1"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -52423,33 +52306,33 @@
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField dataField="1" subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisPage" subtotalTop="0" showAll="0">
+    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisPage" subtotalTop="0" multipleItemSelectionAllowed="1" showAll="0">
       <items count="5">
-        <item x="0"/>
-        <item x="2"/>
+        <item h="1" x="0"/>
+        <item h="1" x="2"/>
         <item x="3"/>
-        <item x="1"/>
+        <item h="1" x="1"/>
         <item t="default"/>
       </items>
     </pivotField>
     <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField subtotalTop="0" showAll="0"/>
@@ -52462,19 +52345,41 @@
     <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0"/>
     <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0"/>
   </pivotFields>
-  <rowItems count="1">
-    <i/>
+  <rowFields count="1">
+    <field x="10"/>
+  </rowFields>
+  <rowItems count="4">
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
   </rowItems>
-  <colItems count="1">
-    <i/>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
   </colItems>
-  <pageFields count="3">
-    <pageField fld="32" item="2" hier="-1"/>
+  <pageFields count="2">
+    <pageField fld="32" hier="-1"/>
     <pageField fld="1" hier="-1"/>
-    <pageField fld="10" item="2" hier="-1"/>
   </pageFields>
-  <dataFields count="1">
-    <dataField name="Sum of Epic Total Estimate" fld="15" baseField="0" baseItem="514"/>
+  <dataFields count="2">
+    <dataField name="Sum of Epic Total Estimate" fld="15" baseField="10" baseItem="0"/>
+    <dataField name="Sum of Epic Remaining Estimate" fld="16" baseField="10" baseItem="0"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -52489,7 +52394,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable20.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="102" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
   <location ref="B29:C44" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="4" colPageCount="1"/>
   <pivotFields count="46">
     <pivotField dataField="1" subtotalTop="0" showAll="0"/>
@@ -52742,8 +52647,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="102" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="9">
-  <location ref="A24:B29" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable8" cacheId="12" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+  <location ref="G35:G36" firstHeaderRow="1" firstDataRow="1" firstDataCol="0" rowPageCount="3" colPageCount="1"/>
   <pivotFields count="46">
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField axis="axisPage" subtotalTop="0" multipleItemSelectionAllowed="1" showAll="0">
@@ -52766,7 +52671,395 @@
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisPage" subtotalTop="0" showAll="0">
+      <items count="5">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisPage" subtotalTop="0" showAll="0">
+      <items count="5">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0"/>
+  </pivotFields>
+  <rowItems count="1">
+    <i/>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <pageFields count="3">
+    <pageField fld="32" item="2" hier="-1"/>
+    <pageField fld="1" hier="-1"/>
+    <pageField fld="10" item="1" hier="-1"/>
+  </pageFields>
+  <dataFields count="1">
+    <dataField name="Sum of Epic Total Estimate" fld="15" baseField="0" baseItem="514"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable10" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
+  <location ref="A49:B54" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
+  <pivotFields count="46">
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisPage" subtotalTop="0" showAll="0">
+      <items count="8">
+        <item x="0"/>
+        <item x="6"/>
+        <item x="2"/>
+        <item x="4"/>
+        <item x="3"/>
+        <item x="5"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisPage" subtotalTop="0" showAll="0">
+      <items count="5">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisRow" subtotalTop="0" showAll="0">
+      <items count="7">
+        <item h="1" x="0"/>
+        <item h="1" x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField subtotalTop="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="35"/>
+  </rowFields>
+  <rowItems count="5">
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <pageFields count="2">
+    <pageField fld="1" item="2" hier="-1"/>
+    <pageField fld="32" item="2" hier="-1"/>
+  </pageFields>
+  <dataFields count="1">
+    <dataField name="Sum of Epic Total Estimate" fld="15" baseField="35" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="5">
+    <chartFormat chart="2" format="10" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="11">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="35" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="12">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="35" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="13">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="35" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="14">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="35" count="1" selected="0">
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="12" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+  <location ref="A34:A35" firstHeaderRow="1" firstDataRow="1" firstDataCol="0" rowPageCount="2" colPageCount="1"/>
+  <pivotFields count="46">
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisPage" subtotalTop="0" multipleItemSelectionAllowed="1" showAll="0">
+      <items count="8">
+        <item h="1" x="0"/>
+        <item h="1" x="6"/>
+        <item x="2"/>
+        <item h="1" x="4"/>
+        <item h="1" x="3"/>
+        <item h="1" x="5"/>
+        <item h="1" x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisPage" subtotalTop="0" showAll="0">
+      <items count="5">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0"/>
+  </pivotFields>
+  <rowItems count="1">
+    <i/>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <pageFields count="2">
+    <pageField fld="32" item="2" hier="-1"/>
+    <pageField fld="1" hier="-1"/>
+  </pageFields>
+  <dataFields count="1">
+    <dataField name="Sum of Epic Total Estimate" fld="15" baseField="0" baseItem="514"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable9" cacheId="12" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="15">
+  <location ref="G24:H29" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
+  <pivotFields count="46">
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisPage" subtotalTop="0" multipleItemSelectionAllowed="1" showAll="0">
+      <items count="8">
+        <item h="1" x="0"/>
+        <item h="1" x="6"/>
+        <item x="2"/>
+        <item h="1" x="4"/>
+        <item h="1" x="3"/>
+        <item h="1" x="5"/>
+        <item h="1" x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisPage" subtotalTop="0" showAll="0">
+      <items count="5">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField subtotalTop="0" showAll="0"/>
@@ -52834,9 +53127,10 @@
   <colItems count="1">
     <i/>
   </colItems>
-  <pageFields count="2">
+  <pageFields count="3">
     <pageField fld="32" item="2" hier="-1"/>
     <pageField fld="1" hier="-1"/>
+    <pageField fld="10" item="1" hier="-1"/>
   </pageFields>
   <dataFields count="5">
     <dataField name="Done" fld="44" baseField="0" baseItem="32"/>
@@ -52845,7 +53139,7 @@
     <dataField name="Ready" fld="39" baseField="0" baseItem="32"/>
     <dataField name="Not Decomposed" fld="45" baseField="0" baseItem="32"/>
   </dataFields>
-  <chartFormats count="15">
+  <chartFormats count="27">
     <chartFormat chart="0" format="7" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="2">
@@ -52987,235 +53281,7 @@
         </references>
       </pivotArea>
     </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable8" cacheId="102" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
-  <location ref="G35:G36" firstHeaderRow="1" firstDataRow="1" firstDataCol="0" rowPageCount="3" colPageCount="1"/>
-  <pivotFields count="46">
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisPage" subtotalTop="0" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="8">
-        <item h="1" x="0"/>
-        <item h="1" x="6"/>
-        <item x="2"/>
-        <item h="1" x="4"/>
-        <item h="1" x="3"/>
-        <item h="1" x="5"/>
-        <item h="1" x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisPage" subtotalTop="0" showAll="0">
-      <items count="5">
-        <item x="0"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisPage" subtotalTop="0" showAll="0">
-      <items count="5">
-        <item x="0"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0"/>
-    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0"/>
-  </pivotFields>
-  <rowItems count="1">
-    <i/>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <pageFields count="3">
-    <pageField fld="32" item="2" hier="-1"/>
-    <pageField fld="1" hier="-1"/>
-    <pageField fld="10" item="1" hier="-1"/>
-  </pageFields>
-  <dataFields count="1">
-    <dataField name="Sum of Epic Total Estimate" fld="15" baseField="0" baseItem="514"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable10" cacheId="102" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
-  <location ref="A49:B54" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
-  <pivotFields count="46">
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisPage" subtotalTop="0" showAll="0">
-      <items count="8">
-        <item x="0"/>
-        <item x="6"/>
-        <item x="2"/>
-        <item x="4"/>
-        <item x="3"/>
-        <item x="5"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisPage" subtotalTop="0" showAll="0">
-      <items count="5">
-        <item x="0"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisRow" subtotalTop="0" showAll="0">
-      <items count="7">
-        <item h="1" x="0"/>
-        <item h="1" x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField subtotalTop="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="35"/>
-  </rowFields>
-  <rowItems count="5">
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <pageFields count="2">
-    <pageField fld="1" item="2" hier="-1"/>
-    <pageField fld="32" item="2" hier="-1"/>
-  </pageFields>
-  <dataFields count="1">
-    <dataField name="Sum of Epic Total Estimate" fld="15" baseField="35" baseItem="0"/>
-  </dataFields>
-  <chartFormats count="5">
-    <chartFormat chart="2" format="10" series="1">
+    <chartFormat chart="7" format="7" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
@@ -53224,50 +53290,101 @@
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="2" format="11">
+    <chartFormat chart="7" format="8">
       <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
+        <references count="1">
           <reference field="4294967294" count="1" selected="0">
             <x v="0"/>
           </reference>
-          <reference field="35" count="1" selected="0">
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="7" format="9">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="7" format="10">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
             <x v="2"/>
           </reference>
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="2" format="12">
+    <chartFormat chart="7" format="11">
       <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
+        <references count="1">
           <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="35" count="1" selected="0">
             <x v="3"/>
           </reference>
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="2" format="13">
+    <chartFormat chart="7" format="12">
       <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
+        <references count="1">
           <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="35" count="1" selected="0">
             <x v="4"/>
           </reference>
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="2" format="14">
+    <chartFormat chart="14" format="19" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
+        <references count="1">
           <reference field="4294967294" count="1" selected="0">
             <x v="0"/>
           </reference>
-          <reference field="35" count="1" selected="0">
-            <x v="5"/>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="14" format="20">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="14" format="21">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="14" format="22">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="14" format="23">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="14" format="24">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="4"/>
           </reference>
         </references>
       </pivotArea>
@@ -53285,9 +53402,9 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="102" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
-  <location ref="A34:A35" firstHeaderRow="1" firstDataRow="1" firstDataCol="0" rowPageCount="2" colPageCount="1"/>
+<file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable5" cacheId="12" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+  <location ref="D35:D36" firstHeaderRow="1" firstDataRow="1" firstDataCol="0" rowPageCount="3" colPageCount="1"/>
   <pivotFields count="46">
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField axis="axisPage" subtotalTop="0" multipleItemSelectionAllowed="1" showAll="0">
@@ -53310,28 +53427,6 @@
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
     <pivotField axis="axisPage" subtotalTop="0" showAll="0">
       <items count="5">
         <item x="0"/>
@@ -53343,6 +53438,36 @@
     </pivotField>
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisPage" subtotalTop="0" showAll="0">
+      <items count="5">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField subtotalTop="0" showAll="0"/>
@@ -53361,9 +53486,10 @@
   <colItems count="1">
     <i/>
   </colItems>
-  <pageFields count="2">
+  <pageFields count="3">
     <pageField fld="32" item="2" hier="-1"/>
     <pageField fld="1" hier="-1"/>
+    <pageField fld="10" item="2" hier="-1"/>
   </pageFields>
   <dataFields count="1">
     <dataField name="Sum of Epic Total Estimate" fld="15" baseField="0" baseItem="514"/>
@@ -53380,8 +53506,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="102" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="12">
+<file path=xl/pivotTables/pivotTable8.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="12" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="12">
   <location ref="D24:E29" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
   <pivotFields count="46">
     <pivotField subtotalTop="0" showAll="0"/>
@@ -53702,134 +53828,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="102" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="Y4:AA8" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
-  <pivotFields count="46">
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisPage" subtotalTop="0" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="8">
-        <item h="1" x="0"/>
-        <item h="1" x="6"/>
-        <item x="2"/>
-        <item h="1" x="4"/>
-        <item h="1" x="3"/>
-        <item h="1" x="5"/>
-        <item h="1" x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisRow" subtotalTop="0" showAll="0">
-      <items count="5">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
-    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisPage" subtotalTop="0" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="5">
-        <item h="1" x="0"/>
-        <item h="1" x="2"/>
-        <item x="3"/>
-        <item h="1" x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0"/>
-    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="10"/>
-  </rowFields>
-  <rowItems count="4">
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="-2"/>
-  </colFields>
-  <colItems count="2">
-    <i>
-      <x/>
-    </i>
-    <i i="1">
-      <x v="1"/>
-    </i>
-  </colItems>
-  <pageFields count="2">
-    <pageField fld="32" hier="-1"/>
-    <pageField fld="1" hier="-1"/>
-  </pageFields>
-  <dataFields count="2">
-    <dataField name="Sum of Epic Total Estimate" fld="15" baseField="10" baseItem="0"/>
-    <dataField name="Sum of Epic Remaining Estimate" fld="16" baseField="10" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
 <file path=xl/pivotTables/pivotTable9.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="102" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="AD10:AH16" firstHeaderRow="1" firstDataRow="3" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="46">
     <pivotField subtotalTop="0" showAll="0"/>
@@ -55347,7 +55347,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -58831,7 +58831,7 @@
     <col min="3" max="3" width="10.19921875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.1328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.9296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.19921875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12" customWidth="1"/>
     <col min="10" max="10" width="9.86328125" customWidth="1"/>
@@ -58895,7 +58895,7 @@
       </c>
       <c r="B2" s="52">
         <f ca="1">MAX(NETWORKDAYS($D$3,$E$6,$W$3:$W$12)/NETWORKDAYS($D$3,$E$3,$W$3:$W$12),0%)</f>
-        <v>0.63793103448275867</v>
+        <v>0.64655172413793105</v>
       </c>
       <c r="D2" s="30" t="s">
         <v>131</v>
@@ -58964,7 +58964,7 @@
       </c>
       <c r="B3" s="32">
         <f ca="1">MAX(100%,B2)-B2</f>
-        <v>0.36206896551724133</v>
+        <v>0.35344827586206895</v>
       </c>
       <c r="D3" s="28">
         <v>43201</v>
@@ -58989,8 +58989,8 @@
         <v>0</v>
       </c>
       <c r="P3" s="46">
-        <f>2350*(100%-K3)</f>
-        <v>2350</v>
+        <f>2380*(100%-K3)</f>
+        <v>2380</v>
       </c>
       <c r="Q3" s="46">
         <v>2023</v>
@@ -59003,8 +59003,8 @@
         <v>918</v>
       </c>
       <c r="T3" s="46">
-        <f t="shared" ref="T3:T17" si="0">675*(100%-L3)</f>
-        <v>675</v>
+        <f>700*(100%-L3)</f>
+        <v>700</v>
       </c>
       <c r="U3" s="46">
         <v>575</v>
@@ -59028,7 +59028,7 @@
         <v>43207</v>
       </c>
       <c r="J4" s="38">
-        <f t="shared" ref="J4:J17" si="1">NETWORKDAYS(H4,I4,$W$3:$W$12)</f>
+        <f t="shared" ref="J4:J17" si="0">NETWORKDAYS(H4,I4,$W$3:$W$12)</f>
         <v>5</v>
       </c>
       <c r="K4" s="40">
@@ -59049,22 +59049,22 @@
         <v>6.0299999999999999E-2</v>
       </c>
       <c r="P4" s="46">
-        <f t="shared" ref="P4:P17" si="2">2350*(100%-K4)</f>
-        <v>2248.7068965517242</v>
+        <f>2380*(100%-K4)</f>
+        <v>2277.4137931034484</v>
       </c>
       <c r="Q4" s="46">
         <v>2324.5</v>
       </c>
       <c r="R4" s="50">
-        <f t="shared" ref="R4:R17" si="3">1400*(100%-K4)</f>
+        <f t="shared" ref="R4:R17" si="1">1400*(100%-K4)</f>
         <v>1339.655172413793</v>
       </c>
       <c r="S4" s="46">
         <v>1274</v>
       </c>
       <c r="T4" s="46">
-        <f t="shared" si="0"/>
-        <v>645.90517241379314</v>
+        <f>700*(100%-L4)</f>
+        <v>669.82758620689651</v>
       </c>
       <c r="U4" s="46">
         <v>654</v>
@@ -59104,7 +59104,7 @@
         <v>43221</v>
       </c>
       <c r="J5" s="38">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="K5" s="40">
@@ -59125,22 +59125,22 @@
         <v>0.18529999999999999</v>
       </c>
       <c r="P5" s="46">
-        <f t="shared" si="2"/>
-        <v>2046.1206896551726</v>
+        <f>2380*(100%-K5)</f>
+        <v>2072.2413793103447</v>
       </c>
       <c r="Q5" s="46">
         <v>2399.3000000000002</v>
       </c>
       <c r="R5" s="50">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>1218.9655172413793</v>
       </c>
       <c r="S5" s="46">
         <v>1544.3</v>
       </c>
       <c r="T5" s="46">
-        <f t="shared" si="0"/>
-        <v>587.7155172413793</v>
+        <f>700*(100%-L5)</f>
+        <v>609.48275862068965</v>
       </c>
       <c r="U5" s="46">
         <v>525.5</v>
@@ -59170,7 +59170,7 @@
       </c>
       <c r="E6" s="27">
         <f ca="1">TODAY()</f>
-        <v>43313</v>
+        <v>43314</v>
       </c>
       <c r="G6" s="23" t="s">
         <v>151</v>
@@ -59184,7 +59184,7 @@
         <v>43235</v>
       </c>
       <c r="J6" s="38">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="K6" s="40">
@@ -59205,22 +59205,22 @@
         <v>0.30580000000000002</v>
       </c>
       <c r="P6" s="46">
-        <f t="shared" si="2"/>
-        <v>1843.5344827586209</v>
+        <f>2380*(100%-K6)</f>
+        <v>1867.0689655172416</v>
       </c>
       <c r="Q6" s="47">
         <v>1859.5</v>
       </c>
       <c r="R6" s="50">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>1098.2758620689656</v>
       </c>
       <c r="S6" s="47">
         <v>1267.5</v>
       </c>
       <c r="T6" s="46">
-        <f t="shared" si="0"/>
-        <v>529.52586206896558</v>
+        <f>700*(100%-L6)</f>
+        <v>549.13793103448279</v>
       </c>
       <c r="U6" s="47">
         <v>462</v>
@@ -59252,15 +59252,15 @@
         <v>152</v>
       </c>
       <c r="H7" s="24">
-        <f t="shared" ref="H7:H17" si="4">I6+1</f>
+        <f t="shared" ref="H7:H17" si="2">I6+1</f>
         <v>43236</v>
       </c>
       <c r="I7" s="24">
-        <f t="shared" ref="I7:I16" si="5">I6+14</f>
+        <f t="shared" ref="I7:I16" si="3">I6+14</f>
         <v>43249</v>
       </c>
       <c r="J7" s="38">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="K7" s="40">
@@ -59281,22 +59281,22 @@
         <v>0.376</v>
       </c>
       <c r="P7" s="46">
-        <f t="shared" si="2"/>
-        <v>1661.206896551724</v>
+        <f>2380*(100%-K7)</f>
+        <v>1682.4137931034481</v>
       </c>
       <c r="Q7" s="47">
         <v>1741</v>
       </c>
       <c r="R7" s="50">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>989.65517241379303</v>
       </c>
       <c r="S7" s="47">
         <v>1161</v>
       </c>
       <c r="T7" s="46">
-        <f t="shared" si="0"/>
-        <v>477.15517241379308</v>
+        <f>700*(100%-L7)</f>
+        <v>494.82758620689651</v>
       </c>
       <c r="U7" s="47">
         <v>458</v>
@@ -59321,15 +59321,15 @@
         <v>153</v>
       </c>
       <c r="H8" s="24">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>43250</v>
       </c>
       <c r="I8" s="24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>43263</v>
       </c>
       <c r="J8" s="38">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="K8" s="40">
@@ -59350,22 +59350,22 @@
         <v>0.43969999999999998</v>
       </c>
       <c r="P8" s="46">
-        <f t="shared" si="2"/>
-        <v>1458.6206896551726</v>
+        <f>2380*(100%-K8)</f>
+        <v>1477.2413793103449</v>
       </c>
       <c r="Q8" s="47">
         <v>1597</v>
       </c>
       <c r="R8" s="50">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>868.9655172413793</v>
       </c>
       <c r="S8" s="47">
         <v>1032.5</v>
       </c>
       <c r="T8" s="46">
-        <f t="shared" si="0"/>
-        <v>418.9655172413793</v>
+        <f>700*(100%-L8)</f>
+        <v>434.48275862068965</v>
       </c>
       <c r="U8" s="47">
         <v>427.5</v>
@@ -59394,15 +59394,15 @@
         <v>154</v>
       </c>
       <c r="H9" s="24">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>43264</v>
       </c>
       <c r="I9" s="24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>43277</v>
       </c>
       <c r="J9" s="38">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="K9" s="40">
@@ -59423,22 +59423,22 @@
         <v>0.57920000000000005</v>
       </c>
       <c r="P9" s="46">
-        <f t="shared" ref="P9" si="6">2350*(100%-K9)</f>
-        <v>1256.0344827586209</v>
+        <f>2380*(100%-K9)</f>
+        <v>1272.0689655172416</v>
       </c>
       <c r="Q9" s="47">
         <v>1184.5</v>
       </c>
       <c r="R9" s="50">
-        <f t="shared" ref="R9" si="7">1400*(100%-K9)</f>
+        <f t="shared" ref="R9" si="4">1400*(100%-K9)</f>
         <v>748.27586206896558</v>
       </c>
       <c r="S9" s="47">
         <v>743.5</v>
       </c>
       <c r="T9" s="46">
-        <f t="shared" si="0"/>
-        <v>360.77586206896558</v>
+        <f>700*(100%-L9)</f>
+        <v>374.13793103448279</v>
       </c>
       <c r="U9" s="47">
         <v>321.5</v>
@@ -59467,7 +59467,7 @@
         <v>43291</v>
       </c>
       <c r="J10" s="38">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="K10" s="40">
@@ -59488,22 +59488,22 @@
         <v>0.67889999999999995</v>
       </c>
       <c r="P10" s="46">
-        <f t="shared" si="2"/>
-        <v>1073.706896551724</v>
+        <f>2380*(100%-K10)</f>
+        <v>1087.4137931034481</v>
       </c>
       <c r="Q10" s="47">
         <v>1001</v>
       </c>
       <c r="R10" s="50">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>639.65517241379303</v>
       </c>
       <c r="S10" s="47">
         <v>634</v>
       </c>
       <c r="T10" s="46">
-        <f t="shared" si="0"/>
-        <v>308.40517241379308</v>
+        <f>700*(100%-L10)</f>
+        <v>319.82758620689651</v>
       </c>
       <c r="U10" s="47">
         <v>249.5</v>
@@ -59524,7 +59524,7 @@
         <v>156</v>
       </c>
       <c r="H11" s="24">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>43292</v>
       </c>
       <c r="I11" s="24">
@@ -59532,7 +59532,7 @@
         <v>43298</v>
       </c>
       <c r="J11" s="38">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K11" s="40">
@@ -59553,22 +59553,22 @@
         <v>0.67030000000000001</v>
       </c>
       <c r="P11" s="46">
-        <f t="shared" si="2"/>
-        <v>1073.706896551724</v>
+        <f>2380*(100%-K11)</f>
+        <v>1087.4137931034481</v>
       </c>
       <c r="Q11" s="47">
         <v>910</v>
       </c>
       <c r="R11" s="50">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>639.65517241379303</v>
       </c>
       <c r="S11" s="47">
         <v>526.5</v>
       </c>
       <c r="T11" s="46">
-        <f t="shared" si="0"/>
-        <v>308.40517241379308</v>
+        <f>700*(100%-L11)</f>
+        <v>319.82758620689651</v>
       </c>
       <c r="U11" s="47">
         <v>259.5</v>
@@ -59582,15 +59582,15 @@
         <v>157</v>
       </c>
       <c r="H12" s="24">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>43299</v>
       </c>
       <c r="I12" s="24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>43312</v>
       </c>
       <c r="J12" s="38">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="K12" s="40">
@@ -59611,22 +59611,22 @@
         <v>0.70540000000000003</v>
       </c>
       <c r="P12" s="46">
-        <f t="shared" si="2"/>
-        <v>871.12068965517244</v>
+        <f>2380*(100%-K12)</f>
+        <v>882.24137931034488</v>
       </c>
       <c r="Q12" s="47">
         <v>793</v>
       </c>
       <c r="R12" s="50">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>518.9655172413793</v>
       </c>
       <c r="S12" s="47">
         <v>401.5</v>
       </c>
       <c r="T12" s="46">
-        <f t="shared" si="0"/>
-        <v>250.21551724137933</v>
+        <f>700*(100%-L12)</f>
+        <v>259.48275862068965</v>
       </c>
       <c r="U12" s="47">
         <v>257</v>
@@ -59643,15 +59643,15 @@
         <v>158</v>
       </c>
       <c r="H13" s="24">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>43313</v>
       </c>
       <c r="I13" s="24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>43326</v>
       </c>
       <c r="J13" s="38">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="K13" s="40">
@@ -59675,15 +59675,15 @@
         <v>0.25</v>
       </c>
       <c r="P13" s="46">
-        <f t="shared" si="2"/>
-        <v>688.79310344827593</v>
+        <f>2380*(100%-K13)</f>
+        <v>697.58620689655174</v>
       </c>
       <c r="Q13" s="47">
         <f>GETPIVOTDATA("Epic Remaining Estimate",$Y$4)</f>
         <v>300</v>
       </c>
       <c r="R13" s="50">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>410.34482758620692</v>
       </c>
       <c r="S13" s="47">
@@ -59691,8 +59691,8 @@
         <v>150</v>
       </c>
       <c r="T13" s="46">
-        <f t="shared" si="0"/>
-        <v>197.84482758620692</v>
+        <f>700*(100%-L13)</f>
+        <v>205.17241379310346</v>
       </c>
       <c r="U13" s="47">
         <f>GETPIVOTDATA("Epic Remaining Estimate",$Y$4,"ST:Components","Artifact List")</f>
@@ -59711,15 +59711,15 @@
         <v>159</v>
       </c>
       <c r="H14" s="24">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>43327</v>
       </c>
       <c r="I14" s="24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>43340</v>
       </c>
       <c r="J14" s="38">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="K14" s="40">
@@ -59734,18 +59734,18 @@
       <c r="N14" s="40"/>
       <c r="O14" s="40"/>
       <c r="P14" s="46">
-        <f t="shared" si="2"/>
-        <v>486.20689655172407</v>
+        <f>2380*(100%-K14)</f>
+        <v>492.4137931034482</v>
       </c>
       <c r="Q14" s="47"/>
       <c r="R14" s="50">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>289.65517241379308</v>
       </c>
       <c r="S14" s="47"/>
       <c r="T14" s="46">
-        <f t="shared" si="0"/>
-        <v>139.65517241379308</v>
+        <f>700*(100%-L14)</f>
+        <v>144.82758620689654</v>
       </c>
       <c r="U14" s="47"/>
     </row>
@@ -59761,15 +59761,15 @@
         <v>160</v>
       </c>
       <c r="H15" s="24">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>43341</v>
       </c>
       <c r="I15" s="24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>43354</v>
       </c>
       <c r="J15" s="38">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="K15" s="40">
@@ -59784,18 +59784,18 @@
       <c r="N15" s="40"/>
       <c r="O15" s="40"/>
       <c r="P15" s="46">
-        <f t="shared" si="2"/>
-        <v>303.87931034482756</v>
+        <f>2380*(100%-K15)</f>
+        <v>307.75862068965512</v>
       </c>
       <c r="Q15" s="47"/>
       <c r="R15" s="50">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>181.03448275862067</v>
       </c>
       <c r="S15" s="47"/>
       <c r="T15" s="46">
-        <f t="shared" si="0"/>
-        <v>87.284482758620683</v>
+        <f>700*(100%-L15)</f>
+        <v>90.517241379310335</v>
       </c>
       <c r="U15" s="47"/>
     </row>
@@ -59804,15 +59804,15 @@
         <v>161</v>
       </c>
       <c r="H16" s="24">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>43355</v>
       </c>
       <c r="I16" s="24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>43368</v>
       </c>
       <c r="J16" s="38">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="K16" s="40">
@@ -59827,18 +59827,18 @@
       <c r="N16" s="40"/>
       <c r="O16" s="40"/>
       <c r="P16" s="46">
-        <f t="shared" si="2"/>
-        <v>101.29310344827593</v>
+        <f>2380*(100%-K16)</f>
+        <v>102.5862068965518</v>
       </c>
       <c r="Q16" s="47"/>
       <c r="R16" s="50">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>60.344827586206939</v>
       </c>
       <c r="S16" s="47"/>
       <c r="T16" s="46">
-        <f t="shared" si="0"/>
-        <v>29.094827586206918</v>
+        <f>700*(100%-L16)</f>
+        <v>30.17241379310347</v>
       </c>
       <c r="U16" s="47"/>
     </row>
@@ -59853,7 +59853,7 @@
         <v>162</v>
       </c>
       <c r="H17" s="26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>43369</v>
       </c>
       <c r="I17" s="26">
@@ -59861,7 +59861,7 @@
         <v>43375</v>
       </c>
       <c r="J17" s="39">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="K17" s="41">
@@ -59876,17 +59876,17 @@
       <c r="N17" s="41"/>
       <c r="O17" s="41"/>
       <c r="P17" s="49">
-        <f t="shared" si="2"/>
+        <f>2380*(100%-K17)</f>
         <v>0</v>
       </c>
       <c r="Q17" s="48"/>
       <c r="R17" s="49">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="S17" s="48"/>
       <c r="T17" s="49">
-        <f t="shared" si="0"/>
+        <f>700*(100%-L17)</f>
         <v>0</v>
       </c>
       <c r="U17" s="48"/>
@@ -59897,7 +59897,7 @@
       </c>
       <c r="B18" s="52">
         <f ca="1">MAX(NETWORKDAYS($D$3,$E$6,$W$3:$W$12)/NETWORKDAYS($D$3,$E$3,$W$3:$W$12),0%)</f>
-        <v>0.63793103448275867</v>
+        <v>0.64655172413793105</v>
       </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.45">
@@ -59906,7 +59906,7 @@
       </c>
       <c r="B19" s="32">
         <f ca="1">MAX(100%,B18)-B18</f>
-        <v>0.36206896551724133</v>
+        <v>0.35344827586206895</v>
       </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.45">
@@ -60479,7 +60479,7 @@
         <v>2023</v>
       </c>
       <c r="E3" s="66">
-        <v>2350</v>
+        <v>2380</v>
       </c>
       <c r="F3" s="46">
         <v>938.5</v>
@@ -60533,7 +60533,7 @@
         <v>575</v>
       </c>
       <c r="U3" s="66">
-        <v>675</v>
+        <v>700</v>
       </c>
       <c r="V3" s="46">
         <v>350</v>
@@ -60571,7 +60571,7 @@
         <v>2442</v>
       </c>
       <c r="E4" s="66">
-        <v>2350</v>
+        <v>2380</v>
       </c>
       <c r="F4" s="46">
         <v>1008</v>
@@ -60623,7 +60623,7 @@
         <v>696</v>
       </c>
       <c r="U4" s="66">
-        <v>675</v>
+        <v>700</v>
       </c>
       <c r="V4" s="46">
         <v>389</v>
@@ -60660,7 +60660,7 @@
         <v>2743.8</v>
       </c>
       <c r="E5" s="66">
-        <v>2350</v>
+        <v>2380</v>
       </c>
       <c r="F5" s="46">
         <v>2218.3000000000002</v>
@@ -60712,7 +60712,7 @@
         <v>645</v>
       </c>
       <c r="U5" s="66">
-        <v>675</v>
+        <v>700</v>
       </c>
       <c r="V5" s="46">
         <v>615</v>
@@ -60749,7 +60749,7 @@
         <v>2412</v>
       </c>
       <c r="E6" s="66">
-        <v>2350</v>
+        <v>2380</v>
       </c>
       <c r="F6" s="46">
         <v>2128.5</v>
@@ -60803,7 +60803,7 @@
         <v>665.5</v>
       </c>
       <c r="U6" s="66">
-        <v>675</v>
+        <v>700</v>
       </c>
       <c r="V6">
         <v>635.5</v>
@@ -60841,7 +60841,7 @@
         <v>2437.5</v>
       </c>
       <c r="E7" s="66">
-        <v>2350</v>
+        <v>2380</v>
       </c>
       <c r="F7" s="46">
         <v>2265</v>
@@ -60895,7 +60895,7 @@
         <v>734</v>
       </c>
       <c r="U7" s="66">
-        <v>675</v>
+        <v>700</v>
       </c>
       <c r="V7" s="46">
         <v>707</v>
@@ -60933,7 +60933,7 @@
         <v>2462.5</v>
       </c>
       <c r="E8" s="66">
-        <v>2350</v>
+        <v>2380</v>
       </c>
       <c r="F8" s="46">
         <v>2354.5</v>
@@ -60987,7 +60987,7 @@
         <v>763</v>
       </c>
       <c r="U8" s="66">
-        <v>675</v>
+        <v>700</v>
       </c>
       <c r="V8" s="46">
         <v>726</v>
@@ -61031,7 +61031,7 @@
         <v>2257</v>
       </c>
       <c r="E9" s="66">
-        <v>2350</v>
+        <v>2380</v>
       </c>
       <c r="F9" s="46">
         <v>2157.5</v>
@@ -61085,7 +61085,7 @@
         <v>764</v>
       </c>
       <c r="U9" s="66">
-        <v>675</v>
+        <v>700</v>
       </c>
       <c r="V9" s="46">
         <v>733</v>
@@ -61123,7 +61123,7 @@
         <v>2264.5</v>
       </c>
       <c r="E10" s="66">
-        <v>2350</v>
+        <v>2380</v>
       </c>
       <c r="F10" s="46">
         <v>2177</v>
@@ -61177,7 +61177,7 @@
         <v>777</v>
       </c>
       <c r="U10" s="66">
-        <v>675</v>
+        <v>700</v>
       </c>
       <c r="V10" s="46">
         <v>755</v>
@@ -61218,7 +61218,7 @@
         <v>2220.5</v>
       </c>
       <c r="E11" s="66">
-        <v>2350</v>
+        <v>2380</v>
       </c>
       <c r="F11" s="46">
         <v>2144</v>
@@ -61272,7 +61272,7 @@
         <v>787</v>
       </c>
       <c r="U11" s="66">
-        <v>675</v>
+        <v>700</v>
       </c>
       <c r="V11" s="46">
         <v>777</v>
@@ -61313,7 +61313,7 @@
         <v>2306.5</v>
       </c>
       <c r="E12" s="66">
-        <v>2350</v>
+        <v>2380</v>
       </c>
       <c r="F12" s="46">
         <v>2212</v>
@@ -61367,7 +61367,7 @@
         <v>872.5</v>
       </c>
       <c r="U12" s="66">
-        <v>675</v>
+        <v>700</v>
       </c>
       <c r="V12" s="46">
         <v>822.5</v>
@@ -61421,7 +61421,7 @@
         <v>1200</v>
       </c>
       <c r="E13" s="66">
-        <v>2350</v>
+        <v>2380</v>
       </c>
       <c r="F13" s="46">
         <f>GETPIVOTDATA("Stories Estimate", $AD$8, "Type", "Epic")</f>
@@ -61483,7 +61483,7 @@
         <v>200</v>
       </c>
       <c r="U13" s="66">
-        <v>675</v>
+        <v>700</v>
       </c>
       <c r="V13" s="46">
         <f>GETPIVOTDATA("Stories Estimate", $AD$8, "Type", "Epic", "ST:Components", "Artifact List")</f>
@@ -61534,13 +61534,13 @@
         <v>43340</v>
       </c>
       <c r="E14" s="66">
-        <v>2350</v>
+        <v>2380</v>
       </c>
       <c r="M14" s="66">
         <v>1400</v>
       </c>
       <c r="U14" s="66">
-        <v>675</v>
+        <v>700</v>
       </c>
       <c r="AD14" s="17" t="s">
         <v>226</v>
@@ -61567,13 +61567,13 @@
         <v>43354</v>
       </c>
       <c r="E15" s="66">
-        <v>2350</v>
+        <v>2380</v>
       </c>
       <c r="M15" s="66">
         <v>1400</v>
       </c>
       <c r="U15" s="66">
-        <v>675</v>
+        <v>700</v>
       </c>
       <c r="AD15" s="17" t="s">
         <v>238</v>
@@ -61596,13 +61596,13 @@
         <v>43368</v>
       </c>
       <c r="E16" s="66">
-        <v>2350</v>
+        <v>2380</v>
       </c>
       <c r="M16" s="66">
         <v>1400</v>
       </c>
       <c r="U16" s="66">
-        <v>675</v>
+        <v>700</v>
       </c>
       <c r="AD16" s="17" t="s">
         <v>50</v>
@@ -61629,13 +61629,13 @@
         <v>43382</v>
       </c>
       <c r="E17" s="66">
-        <v>2350</v>
+        <v>2380</v>
       </c>
       <c r="M17" s="66">
         <v>1400</v>
       </c>
       <c r="U17" s="66">
-        <v>675</v>
+        <v>700</v>
       </c>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.45">
@@ -61656,7 +61656,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -61675,8 +61675,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="16.86328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.06640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.33203125" customWidth="1"/>
     <col min="5" max="5" width="9.46484375" customWidth="1"/>
     <col min="6" max="6" width="8.19921875" bestFit="1" customWidth="1"/>
@@ -61851,11 +61851,11 @@
         <v>158</v>
       </c>
       <c r="C30">
-        <f t="shared" ref="C29:C30" si="0">GETPIVOTDATA("Epic Not Decomposed Estimate",$B$3)</f>
+        <f t="shared" ref="C30" si="0">GETPIVOTDATA("Epic Not Decomposed Estimate",$B$3)</f>
         <v>840</v>
       </c>
       <c r="D30">
-        <f t="shared" ref="D29:D30" si="1">GETPIVOTDATA("Story Points",$B$12)</f>
+        <f t="shared" ref="D30" si="1">GETPIVOTDATA("Story Points",$B$12)</f>
         <v>150</v>
       </c>
     </row>
@@ -61891,7 +61891,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -61907,7 +61907,7 @@
   <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pivotSelection pane="bottomRight" click="1" r:id="rId1">
+      <pivotSelection pane="bottomRight" click="1" r:id="rId3">
         <pivotArea field="32" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisPage" fieldPosition="0"/>
       </pivotSelection>
     </sheetView>

</xml_diff>

<commit_message>
Fixed Artifact List cumulative diagram.
</commit_message>
<xml_diff>
--- a/blueprint-jira-better-excel/_Current-Release-Dashboard.xlsx
+++ b/blueprint-jira-better-excel/_Current-Release-Dashboard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\etc\blueprint-jira-better-excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:180000_{2CE9D2A8-A721-4975-990B-1F44C20F1614}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:180000_{654CE6D7-E04B-4A8B-819D-5C6B28BBBDF7}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="8715" tabRatio="933" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
   </definedNames>
   <calcPr calcId="179017"/>
   <pivotCaches>
-    <pivotCache cacheId="54" r:id="rId18"/>
+    <pivotCache cacheId="13" r:id="rId18"/>
   </pivotCaches>
   <fileRecoveryPr autoRecover="0"/>
 </workbook>
@@ -1776,10 +1776,10 @@
                 <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0" formatCode="0%">
-                  <c:v>0.80172413793103448</c:v>
+                  <c:v>0.86206896551724133</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.19827586206896552</c:v>
+                  <c:v>0.13793103448275867</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5288,10 +5288,10 @@
                 <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0" formatCode="0%">
-                  <c:v>0.80172413793103448</c:v>
+                  <c:v>0.86206896551724133</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.19827586206896552</c:v>
+                  <c:v>0.13793103448275867</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7883,10 +7883,10 @@
                   <c:v>944</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>937</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>200</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>937</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8013,10 +8013,10 @@
                   <c:v>874</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>922</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>922</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8145,10 +8145,10 @@
                   <c:v>822.5</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>917</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>180</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>917</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8275,10 +8275,10 @@
                   <c:v>693.5</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>748</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>748</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -25609,10 +25609,10 @@
                 <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0" formatCode="0%">
-                  <c:v>0.80172413793103448</c:v>
+                  <c:v>0.86206896551724133</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.19827586206896552</c:v>
+                  <c:v>0.13793103448275867</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -43300,7 +43300,7 @@
               <a:cs typeface="Calibri"/>
             </a:rPr>
             <a:pPr algn="ctr"/>
-            <a:t>80%</a:t>
+            <a:t>86%</a:t>
           </a:fld>
           <a:endParaRPr lang="en-US" sz="1800" b="1">
             <a:solidFill>
@@ -43976,7 +43976,7 @@
               <a:cs typeface="Calibri"/>
             </a:rPr>
             <a:pPr algn="ctr"/>
-            <a:t>80%</a:t>
+            <a:t>86%</a:t>
           </a:fld>
           <a:endParaRPr lang="en-US" sz="1800" b="1">
             <a:solidFill>
@@ -44483,7 +44483,7 @@
               <a:cs typeface="Calibri"/>
             </a:rPr>
             <a:pPr algn="ctr"/>
-            <a:t>80%</a:t>
+            <a:t>86%</a:t>
           </a:fld>
           <a:endParaRPr lang="en-US" sz="1800" b="1">
             <a:solidFill>
@@ -44500,7 +44500,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Alex Folomechine" refreshedDate="43341.362470138891" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="90" xr:uid="{00000000-000A-0000-FFFF-FFFF0C000000}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Alex Folomechine" refreshedDate="43353.352372569447" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="90" xr:uid="{00000000-000A-0000-FFFF-FFFF0C000000}">
   <cacheSource type="worksheet">
     <worksheetSource name="issues"/>
   </cacheSource>
@@ -49040,8 +49040,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0300-000006000000}" name="PivotTable8" cacheId="54" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
-  <location ref="G35:G36" firstHeaderRow="1" firstDataRow="1" firstDataCol="0" rowPageCount="3" colPageCount="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0300-000005000000}" name="PivotTable5" cacheId="13" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+  <location ref="D35:D36" firstHeaderRow="1" firstDataRow="1" firstDataCol="0" rowPageCount="3" colPageCount="1"/>
   <pivotFields count="47">
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField axis="axisPage" subtotalTop="0" multipleItemSelectionAllowed="1" showAll="0">
@@ -49128,7 +49128,7 @@
   <pageFields count="3">
     <pageField fld="32" item="2" hier="-1"/>
     <pageField fld="1" hier="-1"/>
-    <pageField fld="10" item="1" hier="-1"/>
+    <pageField fld="10" item="2" hier="-1"/>
   </pageFields>
   <dataFields count="1">
     <dataField name="Sum of Epic Total Estimate" fld="15" baseField="0" baseItem="514"/>
@@ -49146,7 +49146,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable10.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0600-000000000000}" name="PivotTable5" cacheId="54" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0600-000000000000}" name="PivotTable5" cacheId="13" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="B3:C5" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="47">
     <pivotField subtotalTop="0" showAll="0"/>
@@ -49238,7 +49238,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable11.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{0D8B9FB5-5471-4500-848C-1623DA7CC3A0}" name="PivotTable4" cacheId="54" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{0D8B9FB5-5471-4500-848C-1623DA7CC3A0}" name="PivotTable4" cacheId="13" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="G4:H7" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
   <pivotFields count="47">
     <pivotField showAll="0"/>
@@ -49360,7 +49360,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable12.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0800-000000000000}" name="PivotTable1" cacheId="54" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="11">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0800-000000000000}" name="PivotTable1" cacheId="13" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="11">
   <location ref="A5:B11" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
   <pivotFields count="47">
     <pivotField subtotalTop="0" showAll="0"/>
@@ -49577,7 +49577,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable13.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0800-000003000000}" name="PivotTable5" cacheId="54" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="15">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0800-000003000000}" name="PivotTable5" cacheId="13" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="15">
   <location ref="J5:K11" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
   <pivotFields count="47">
     <pivotField subtotalTop="0" showAll="0"/>
@@ -50091,7 +50091,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable14.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0800-000002000000}" name="PivotTable4" cacheId="54" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="15">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0800-000002000000}" name="PivotTable4" cacheId="13" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="15">
   <location ref="G5:H11" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
   <pivotFields count="47">
     <pivotField subtotalTop="0" showAll="0"/>
@@ -50605,7 +50605,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable15.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0800-000001000000}" name="PivotTable3" cacheId="54" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="16">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0800-000001000000}" name="PivotTable3" cacheId="13" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="16">
   <location ref="D5:E11" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
   <pivotFields count="47">
     <pivotField subtotalTop="0" showAll="0"/>
@@ -51062,7 +51062,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable16.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0A00-000000000000}" name="PivotTable1" cacheId="54" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0A00-000000000000}" name="PivotTable1" cacheId="13" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
   <location ref="B4:H20" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
   <pivotFields count="47">
     <pivotField subtotalTop="0" showAll="0"/>
@@ -51365,7 +51365,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable17.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0C00-000000000000}" name="PivotTable2" cacheId="54" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0C00-000000000000}" name="PivotTable2" cacheId="13" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="D4:E11" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
   <pivotFields count="47">
     <pivotField subtotalTop="0" showAll="0"/>
@@ -51633,7 +51633,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable18.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0E00-000001000000}" name="PivotTable2" cacheId="54" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0E00-000001000000}" name="PivotTable2" cacheId="13" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="F8:L11" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
   <pivotFields count="47">
     <pivotField dataField="1" subtotalTop="0" showAll="0"/>
@@ -51948,7 +51948,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable19.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0E00-000000000000}" name="PivotTable1" cacheId="54" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="5">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0E00-000000000000}" name="PivotTable1" cacheId="13" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="5">
   <location ref="B9:C15" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="4" colPageCount="1"/>
   <pivotFields count="47">
     <pivotField dataField="1" subtotalTop="0" showAll="0"/>
@@ -52352,8 +52352,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0300-000000000000}" name="PivotTable1" cacheId="54" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="Y4:AA8" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0300-000006000000}" name="PivotTable8" cacheId="13" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+  <location ref="G35:G36" firstHeaderRow="1" firstDataRow="1" firstDataCol="0" rowPageCount="3" colPageCount="1"/>
   <pivotFields count="47">
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField axis="axisPage" subtotalTop="0" multipleItemSelectionAllowed="1" showAll="0">
@@ -52376,12 +52376,12 @@
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisRow" subtotalTop="0" showAll="0">
+    <pivotField axis="axisPage" subtotalTop="0" showAll="0">
       <items count="5">
         <item x="0"/>
-        <item x="1"/>
         <item x="2"/>
         <item x="3"/>
+        <item x="1"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -52390,34 +52390,34 @@
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField dataField="1" subtotalTop="0" showAll="0"/>
-    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisPage" subtotalTop="0" multipleItemSelectionAllowed="1" showAll="0">
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisPage" subtotalTop="0" showAll="0">
       <items count="6">
-        <item h="1" x="0"/>
-        <item h="1" x="2"/>
+        <item x="0"/>
+        <item x="2"/>
         <item x="3"/>
-        <item h="1" x="1"/>
-        <item h="1" x="4"/>
+        <item x="1"/>
+        <item x="4"/>
         <item t="default"/>
       </items>
     </pivotField>
     <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField subtotalTop="0" showAll="0"/>
@@ -52431,41 +52431,19 @@
     <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
     <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
   </pivotFields>
-  <rowFields count="1">
-    <field x="10"/>
-  </rowFields>
-  <rowItems count="4">
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
+  <rowItems count="1">
+    <i/>
   </rowItems>
-  <colFields count="1">
-    <field x="-2"/>
-  </colFields>
-  <colItems count="2">
-    <i>
-      <x/>
-    </i>
-    <i i="1">
-      <x v="1"/>
-    </i>
+  <colItems count="1">
+    <i/>
   </colItems>
-  <pageFields count="2">
-    <pageField fld="32" hier="-1"/>
+  <pageFields count="3">
+    <pageField fld="32" item="2" hier="-1"/>
     <pageField fld="1" hier="-1"/>
+    <pageField fld="10" item="1" hier="-1"/>
   </pageFields>
-  <dataFields count="2">
-    <dataField name="Sum of Epic Total Estimate" fld="15" baseField="10" baseItem="0"/>
-    <dataField name="Sum of Epic Remaining Estimate" fld="16" baseField="10" baseItem="0"/>
+  <dataFields count="1">
+    <dataField name="Sum of Epic Total Estimate" fld="15" baseField="0" baseItem="514"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -52480,7 +52458,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable20.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0E00-000002000000}" name="PivotTable3" cacheId="54" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0E00-000002000000}" name="PivotTable3" cacheId="13" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
   <location ref="B29:C44" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="4" colPageCount="1"/>
   <pivotFields count="47">
     <pivotField dataField="1" subtotalTop="0" showAll="0"/>
@@ -52735,7 +52713,232 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0300-000002000000}" name="PivotTable2" cacheId="54" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="9">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0300-000000000000}" name="PivotTable1" cacheId="13" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="Y4:AA8" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
+  <pivotFields count="47">
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisPage" subtotalTop="0" multipleItemSelectionAllowed="1" showAll="0">
+      <items count="8">
+        <item h="1" x="0"/>
+        <item h="1" x="6"/>
+        <item x="2"/>
+        <item h="1" x="4"/>
+        <item h="1" x="3"/>
+        <item h="1" x="5"/>
+        <item h="1" x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisRow" subtotalTop="0" showAll="0">
+      <items count="5">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
+    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisPage" subtotalTop="0" multipleItemSelectionAllowed="1" showAll="0">
+      <items count="6">
+        <item h="1" x="0"/>
+        <item h="1" x="2"/>
+        <item x="3"/>
+        <item h="1" x="1"/>
+        <item h="1" x="4"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="10"/>
+  </rowFields>
+  <rowItems count="4">
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+  </colItems>
+  <pageFields count="2">
+    <pageField fld="32" hier="-1"/>
+    <pageField fld="1" hier="-1"/>
+  </pageFields>
+  <dataFields count="2">
+    <dataField name="Sum of Epic Total Estimate" fld="15" baseField="10" baseItem="0"/>
+    <dataField name="Sum of Epic Remaining Estimate" fld="16" baseField="10" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0300-000003000000}" name="PivotTable3" cacheId="13" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+  <location ref="A34:A35" firstHeaderRow="1" firstDataRow="1" firstDataCol="0" rowPageCount="2" colPageCount="1"/>
+  <pivotFields count="47">
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisPage" subtotalTop="0" multipleItemSelectionAllowed="1" showAll="0">
+      <items count="8">
+        <item h="1" x="0"/>
+        <item h="1" x="6"/>
+        <item x="2"/>
+        <item h="1" x="4"/>
+        <item h="1" x="3"/>
+        <item h="1" x="5"/>
+        <item h="1" x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisPage" subtotalTop="0" showAll="0">
+      <items count="6">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="1"/>
+        <item x="4"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+  </pivotFields>
+  <rowItems count="1">
+    <i/>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <pageFields count="2">
+    <pageField fld="32" item="2" hier="-1"/>
+    <pageField fld="1" hier="-1"/>
+  </pageFields>
+  <dataFields count="1">
+    <dataField name="Sum of Epic Total Estimate" fld="15" baseField="0" baseItem="514"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0300-000002000000}" name="PivotTable2" cacheId="13" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="9">
   <location ref="A24:B29" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
   <pivotFields count="47">
     <pivotField subtotalTop="0" showAll="0"/>
@@ -52995,718 +53198,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0300-000004000000}" name="PivotTable4" cacheId="54" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="12">
-  <location ref="D24:E29" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
-  <pivotFields count="47">
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisPage" subtotalTop="0" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="8">
-        <item h="1" x="0"/>
-        <item h="1" x="6"/>
-        <item x="2"/>
-        <item h="1" x="4"/>
-        <item h="1" x="3"/>
-        <item h="1" x="5"/>
-        <item h="1" x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisPage" subtotalTop="0" showAll="0">
-      <items count="5">
-        <item x="0"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisPage" subtotalTop="0" showAll="0">
-      <items count="6">
-        <item x="0"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="1"/>
-        <item x="4"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField dataField="1" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="-2"/>
-  </rowFields>
-  <rowItems count="5">
-    <i>
-      <x/>
-    </i>
-    <i i="1">
-      <x v="1"/>
-    </i>
-    <i i="2">
-      <x v="2"/>
-    </i>
-    <i i="3">
-      <x v="3"/>
-    </i>
-    <i i="4">
-      <x v="4"/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <pageFields count="3">
-    <pageField fld="32" item="2" hier="-1"/>
-    <pageField fld="1" hier="-1"/>
-    <pageField fld="10" item="2" hier="-1"/>
-  </pageFields>
-  <dataFields count="5">
-    <dataField name="Done" fld="45" baseField="0" baseItem="32"/>
-    <dataField name="In Validation" fld="41" baseField="0" baseItem="32"/>
-    <dataField name="In Dev" fld="40" baseField="0" baseItem="32"/>
-    <dataField name="Ready" fld="39" baseField="0" baseItem="32"/>
-    <dataField name="Not Decomposed" fld="46" baseField="0" baseItem="32"/>
-  </dataFields>
-  <chartFormats count="21">
-    <chartFormat chart="0" format="7" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="8" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="9" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="10" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="11">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="12">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="13">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="14">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="4"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="15">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="4" format="22" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="4" format="23">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="4" format="24">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="4" format="25">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="4" format="26">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="4" format="27">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="4"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="9" format="19" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="9" format="20">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="9" format="21">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="9" format="22">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="9" format="23">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="9" format="24">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="4"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0300-000001000000}" name="PivotTable10" cacheId="54" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
-  <location ref="A49:B54" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
-  <pivotFields count="47">
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisPage" subtotalTop="0" showAll="0">
-      <items count="8">
-        <item x="0"/>
-        <item x="6"/>
-        <item x="2"/>
-        <item x="4"/>
-        <item x="3"/>
-        <item x="5"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisPage" subtotalTop="0" showAll="0">
-      <items count="6">
-        <item x="0"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="1"/>
-        <item x="4"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisRow" subtotalTop="0" showAll="0">
-      <items count="7">
-        <item h="1" x="0"/>
-        <item h="1" x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField subtotalTop="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField subtotalTop="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="35"/>
-  </rowFields>
-  <rowItems count="5">
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <pageFields count="2">
-    <pageField fld="1" item="2" hier="-1"/>
-    <pageField fld="32" item="2" hier="-1"/>
-  </pageFields>
-  <dataFields count="1">
-    <dataField name="Sum of Epic Total Estimate" fld="15" baseField="35" baseItem="0"/>
-  </dataFields>
-  <chartFormats count="5">
-    <chartFormat chart="2" format="10" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="2" format="11">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="35" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="2" format="12">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="35" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="2" format="13">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="35" count="1" selected="0">
-            <x v="4"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="2" format="14">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="35" count="1" selected="0">
-            <x v="5"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
 <file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0300-000005000000}" name="PivotTable5" cacheId="54" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
-  <location ref="D35:D36" firstHeaderRow="1" firstDataRow="1" firstDataCol="0" rowPageCount="3" colPageCount="1"/>
-  <pivotFields count="47">
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisPage" subtotalTop="0" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="8">
-        <item h="1" x="0"/>
-        <item h="1" x="6"/>
-        <item x="2"/>
-        <item h="1" x="4"/>
-        <item h="1" x="3"/>
-        <item h="1" x="5"/>
-        <item h="1" x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisPage" subtotalTop="0" showAll="0">
-      <items count="5">
-        <item x="0"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisPage" subtotalTop="0" showAll="0">
-      <items count="6">
-        <item x="0"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="1"/>
-        <item x="4"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-  </pivotFields>
-  <rowItems count="1">
-    <i/>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <pageFields count="3">
-    <pageField fld="32" item="2" hier="-1"/>
-    <pageField fld="1" hier="-1"/>
-    <pageField fld="10" item="2" hier="-1"/>
-  </pageFields>
-  <dataFields count="1">
-    <dataField name="Sum of Epic Total Estimate" fld="15" baseField="0" baseItem="514"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0300-000003000000}" name="PivotTable3" cacheId="54" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
-  <location ref="A34:A35" firstHeaderRow="1" firstDataRow="1" firstDataCol="0" rowPageCount="2" colPageCount="1"/>
-  <pivotFields count="47">
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisPage" subtotalTop="0" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="8">
-        <item h="1" x="0"/>
-        <item h="1" x="6"/>
-        <item x="2"/>
-        <item h="1" x="4"/>
-        <item h="1" x="3"/>
-        <item h="1" x="5"/>
-        <item h="1" x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisPage" subtotalTop="0" showAll="0">
-      <items count="6">
-        <item x="0"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="1"/>
-        <item x="4"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-  </pivotFields>
-  <rowItems count="1">
-    <i/>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <pageFields count="2">
-    <pageField fld="32" item="2" hier="-1"/>
-    <pageField fld="1" hier="-1"/>
-  </pageFields>
-  <dataFields count="1">
-    <dataField name="Sum of Epic Total Estimate" fld="15" baseField="0" baseItem="514"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0300-000007000000}" name="PivotTable9" cacheId="54" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="15">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0300-000007000000}" name="PivotTable9" cacheId="13" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="15">
   <location ref="G24:H29" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
   <pivotFields count="47">
     <pivotField subtotalTop="0" showAll="0"/>
@@ -54083,8 +53576,515 @@
 </pivotTableDefinition>
 </file>
 
+<file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0300-000004000000}" name="PivotTable4" cacheId="13" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="12">
+  <location ref="D24:E29" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
+  <pivotFields count="47">
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisPage" subtotalTop="0" multipleItemSelectionAllowed="1" showAll="0">
+      <items count="8">
+        <item h="1" x="0"/>
+        <item h="1" x="6"/>
+        <item x="2"/>
+        <item h="1" x="4"/>
+        <item h="1" x="3"/>
+        <item h="1" x="5"/>
+        <item h="1" x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisPage" subtotalTop="0" showAll="0">
+      <items count="5">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisPage" subtotalTop="0" showAll="0">
+      <items count="6">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="1"/>
+        <item x="4"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dataField="1" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="-2"/>
+  </rowFields>
+  <rowItems count="5">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+    <i i="2">
+      <x v="2"/>
+    </i>
+    <i i="3">
+      <x v="3"/>
+    </i>
+    <i i="4">
+      <x v="4"/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <pageFields count="3">
+    <pageField fld="32" item="2" hier="-1"/>
+    <pageField fld="1" hier="-1"/>
+    <pageField fld="10" item="2" hier="-1"/>
+  </pageFields>
+  <dataFields count="5">
+    <dataField name="Done" fld="45" baseField="0" baseItem="32"/>
+    <dataField name="In Validation" fld="41" baseField="0" baseItem="32"/>
+    <dataField name="In Dev" fld="40" baseField="0" baseItem="32"/>
+    <dataField name="Ready" fld="39" baseField="0" baseItem="32"/>
+    <dataField name="Not Decomposed" fld="46" baseField="0" baseItem="32"/>
+  </dataFields>
+  <chartFormats count="21">
+    <chartFormat chart="0" format="7" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="8" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="9" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="10" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="11">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="12">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="13">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="14">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="15">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="4" format="22" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="4" format="23">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="4" format="24">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="4" format="25">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="4" format="26">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="4" format="27">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="9" format="19" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="9" format="20">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="9" format="21">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="9" format="22">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="9" format="23">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="9" format="24">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable8.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0300-000001000000}" name="PivotTable10" cacheId="13" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
+  <location ref="A49:B54" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
+  <pivotFields count="47">
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisPage" subtotalTop="0" showAll="0">
+      <items count="8">
+        <item x="0"/>
+        <item x="6"/>
+        <item x="2"/>
+        <item x="4"/>
+        <item x="3"/>
+        <item x="5"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisPage" subtotalTop="0" showAll="0">
+      <items count="6">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="1"/>
+        <item x="4"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisRow" subtotalTop="0" showAll="0">
+      <items count="7">
+        <item h="1" x="0"/>
+        <item h="1" x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField subtotalTop="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField subtotalTop="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="35"/>
+  </rowFields>
+  <rowItems count="5">
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <pageFields count="2">
+    <pageField fld="1" item="2" hier="-1"/>
+    <pageField fld="32" item="2" hier="-1"/>
+  </pageFields>
+  <dataFields count="1">
+    <dataField name="Sum of Epic Total Estimate" fld="15" baseField="35" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="5">
+    <chartFormat chart="2" format="10" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="11">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="35" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="12">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="35" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="13">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="35" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="14">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="35" count="1" selected="0">
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
 <file path=xl/pivotTables/pivotTable9.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0400-000000000000}" name="PivotTable1" cacheId="54" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0400-000000000000}" name="PivotTable1" cacheId="13" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="AD10:AH16" firstHeaderRow="1" firstDataRow="3" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="47">
     <pivotField subtotalTop="0" showAll="0"/>
@@ -59147,10 +59147,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="22.9296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.9296875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.19921875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.9296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.1328125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.19921875" bestFit="1" customWidth="1"/>
@@ -59216,7 +59216,7 @@
       </c>
       <c r="B2" s="52">
         <f ca="1">MAX(NETWORKDAYS($D$3,$E$6,$W$3:$W$12)/NETWORKDAYS($D$3,$E$3,$W$3:$W$12),0%)</f>
-        <v>0.80172413793103448</v>
+        <v>0.86206896551724133</v>
       </c>
       <c r="D2" s="30" t="s">
         <v>130</v>
@@ -59285,7 +59285,7 @@
       </c>
       <c r="B3" s="32">
         <f ca="1">MAX(100%,B2)-B2</f>
-        <v>0.19827586206896552</v>
+        <v>0.13793103448275867</v>
       </c>
       <c r="D3" s="28">
         <v>43201</v>
@@ -59491,7 +59491,7 @@
       </c>
       <c r="E6" s="27">
         <f ca="1">TODAY()</f>
-        <v>43341</v>
+        <v>43353</v>
       </c>
       <c r="G6" s="23" t="s">
         <v>150</v>
@@ -60242,7 +60242,7 @@
       </c>
       <c r="B18" s="52">
         <f ca="1">MAX(NETWORKDAYS($D$3,$E$6,$W$3:$W$12)/NETWORKDAYS($D$3,$E$3,$W$3:$W$12),0%)</f>
-        <v>0.80172413793103448</v>
+        <v>0.86206896551724133</v>
       </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.45">
@@ -60251,7 +60251,7 @@
       </c>
       <c r="B19" s="32">
         <f ca="1">MAX(100%,B18)-B18</f>
-        <v>0.19827586206896552</v>
+        <v>0.13793103448275867</v>
       </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.45">
@@ -61921,35 +61921,31 @@
         <v>0.82768496420047732</v>
       </c>
       <c r="T14" s="65">
-        <f>GETPIVOTDATA("Epic Total Estimate", $AD$8, "Type", "Epic", "ST:Components", "Artifact List")</f>
-        <v>200</v>
+        <v>937</v>
       </c>
       <c r="U14" s="66">
         <v>700</v>
       </c>
       <c r="V14" s="46">
-        <f>GETPIVOTDATA("Stories Estimate", $AD$8, "Type", "Epic", "ST:Components", "Artifact List")</f>
-        <v>0</v>
+        <v>922</v>
       </c>
       <c r="W14" s="46">
-        <f>GETPIVOTDATA("Epic Decomposed", $AD$8, "Type", "Epic", "ST:Components", "Artifact List")</f>
-        <v>180</v>
+        <v>917</v>
       </c>
       <c r="X14" s="46">
         <f t="shared" ref="X14" si="34">T14-Y14</f>
-        <v>50</v>
+        <v>748</v>
       </c>
       <c r="Y14" s="46">
-        <f>GETPIVOTDATA("Epic Remaining Estimate", $AD$8, "Type", "Epic", "ST:Components", "Artifact List")</f>
-        <v>150</v>
+        <v>189</v>
       </c>
       <c r="Z14" s="36">
         <f t="shared" ref="Z14" si="35" xml:space="preserve"> W14/T14</f>
-        <v>0.9</v>
+        <v>0.97865528281750269</v>
       </c>
       <c r="AA14" s="36">
         <f t="shared" ref="AA14" si="36">X14/T14</f>
-        <v>0.25</v>
+        <v>0.79829242262540023</v>
       </c>
       <c r="AD14" s="17" t="s">
         <v>225</v>
@@ -62038,31 +62034,35 @@
         <v>0.25</v>
       </c>
       <c r="T15" s="65">
-        <v>937</v>
+        <f>GETPIVOTDATA("Epic Total Estimate", $AD$8, "Type", "Epic", "ST:Components", "Artifact List")</f>
+        <v>200</v>
       </c>
       <c r="U15" s="66">
         <v>700</v>
       </c>
       <c r="V15" s="46">
-        <v>922</v>
+        <f>GETPIVOTDATA("Stories Estimate", $AD$8, "Type", "Epic", "ST:Components", "Artifact List")</f>
+        <v>0</v>
       </c>
       <c r="W15" s="46">
-        <v>917</v>
+        <f>GETPIVOTDATA("Epic Decomposed", $AD$8, "Type", "Epic", "ST:Components", "Artifact List")</f>
+        <v>180</v>
       </c>
       <c r="X15" s="46">
         <f t="shared" ref="X15" si="43">T15-Y15</f>
-        <v>748</v>
+        <v>50</v>
       </c>
       <c r="Y15" s="46">
-        <v>189</v>
+        <f>GETPIVOTDATA("Epic Remaining Estimate", $AD$8, "Type", "Epic", "ST:Components", "Artifact List")</f>
+        <v>150</v>
       </c>
       <c r="Z15" s="36">
         <f t="shared" ref="Z15" si="44" xml:space="preserve"> W15/T15</f>
-        <v>0.97865528281750269</v>
+        <v>0.9</v>
       </c>
       <c r="AA15" s="36">
         <f t="shared" ref="AA15" si="45">X15/T15</f>
-        <v>0.79829242262540023</v>
+        <v>0.25</v>
       </c>
       <c r="AD15" s="17" t="s">
         <v>237</v>
@@ -62380,7 +62380,7 @@
         <v>159</v>
       </c>
       <c r="C27">
-        <f t="shared" ref="C26:C27" si="0">GETPIVOTDATA("Epic Not Decomposed Estimate",$B$3)</f>
+        <f t="shared" ref="C27" si="0">GETPIVOTDATA("Epic Not Decomposed Estimate",$B$3)</f>
         <v>840</v>
       </c>
       <c r="D27">

</xml_diff>